<commit_message>
end make all wells
</commit_message>
<xml_diff>
--- a/types/j.xlsx
+++ b/types/j.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,40 +434,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>md</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>inclination</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>azimuth</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>z</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -476,272 +476,266 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B3" t="n">
         <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1000</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="n">
+        <v>1031</v>
       </c>
       <c r="B4" t="n">
-        <v>1030</v>
+        <v>5.399999999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>3.375</v>
-      </c>
-      <c r="D4" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="n">
+        <v>1061</v>
       </c>
       <c r="B5" t="n">
-        <v>1060</v>
+        <v>10.8</v>
       </c>
       <c r="C5" t="n">
-        <v>6.75</v>
-      </c>
-      <c r="D5" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" t="n">
+        <v>1091</v>
       </c>
       <c r="B6" t="n">
-        <v>1090</v>
+        <v>16.2</v>
       </c>
       <c r="C6" t="n">
-        <v>10.125</v>
-      </c>
-      <c r="D6" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" t="n">
+        <v>1121</v>
       </c>
       <c r="B7" t="n">
-        <v>1120</v>
+        <v>21.6</v>
       </c>
       <c r="C7" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" t="n">
+        <v>1151</v>
       </c>
       <c r="B8" t="n">
-        <v>1150</v>
+        <v>27</v>
       </c>
       <c r="C8" t="n">
-        <v>16.875</v>
-      </c>
-      <c r="D8" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" t="n">
+        <v>1181</v>
       </c>
       <c r="B9" t="n">
-        <v>1180</v>
+        <v>32.4</v>
       </c>
       <c r="C9" t="n">
-        <v>20.25</v>
-      </c>
-      <c r="D9" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" t="n">
+        <v>1211</v>
       </c>
       <c r="B10" t="n">
-        <v>1210</v>
+        <v>37.8</v>
       </c>
       <c r="C10" t="n">
-        <v>23.625</v>
-      </c>
-      <c r="D10" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" t="n">
+        <v>1241</v>
       </c>
       <c r="B11" t="n">
-        <v>1240</v>
+        <v>43.2</v>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
-      </c>
-      <c r="D11" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
+      <c r="A12" t="n">
+        <v>1271</v>
       </c>
       <c r="B12" t="n">
-        <v>1270</v>
+        <v>48.59999999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>30.375</v>
-      </c>
-      <c r="D12" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
+      <c r="A13" t="n">
+        <v>1301</v>
       </c>
       <c r="B13" t="n">
-        <v>1300</v>
+        <v>53.99999999999999</v>
       </c>
       <c r="C13" t="n">
-        <v>33.75</v>
-      </c>
-      <c r="D13" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
+      <c r="A14" t="n">
+        <v>1331</v>
       </c>
       <c r="B14" t="n">
-        <v>1330</v>
+        <v>59.39999999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>37.125</v>
-      </c>
-      <c r="D14" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
+      <c r="A15" t="n">
+        <v>1361</v>
       </c>
       <c r="B15" t="n">
-        <v>1360</v>
+        <v>64.8</v>
       </c>
       <c r="C15" t="n">
-        <v>40.5</v>
-      </c>
-      <c r="D15" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
+      <c r="A16" t="n">
+        <v>1391</v>
       </c>
       <c r="B16" t="n">
-        <v>1390</v>
+        <v>70.19999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>43.875</v>
-      </c>
-      <c r="D16" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
+      <c r="A17" t="n">
+        <v>1421</v>
       </c>
       <c r="B17" t="n">
-        <v>1390</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>45</v>
-      </c>
-      <c r="D17" t="n">
-        <v>90</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1451</v>
+      </c>
+      <c r="B18" t="n">
+        <v>80.99999999999999</v>
+      </c>
+      <c r="C18" t="n">
+        <v>123</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1481</v>
+      </c>
+      <c r="B19" t="n">
+        <v>86.39999999999999</v>
+      </c>
+      <c r="C19" t="n">
+        <v>123</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1881</v>
+      </c>
+      <c r="B20" t="n">
+        <v>90</v>
+      </c>
+      <c r="C20" t="n">
+        <v>123</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>